<commit_message>
Worked on HSV ROC curves and models
</commit_message>
<xml_diff>
--- a/data/03_first_25percent_metrics/color_and_spatial_metrics_agg.xlsx
+++ b/data/03_first_25percent_metrics/color_and_spatial_metrics_agg.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:BU9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,7 +465,7 @@
       <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Ranks</t>
+          <t>Labels</t>
         </is>
       </c>
       <c r="C1" s="1" t="n"/>
@@ -473,16 +473,16 @@
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Ranks</t>
+        </is>
+      </c>
       <c r="I1" s="1" t="n"/>
       <c r="J1" s="1" t="n"/>
       <c r="K1" s="1" t="n"/>
       <c r="L1" s="1" t="n"/>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Values</t>
-        </is>
-      </c>
+      <c r="M1" s="1" t="n"/>
       <c r="N1" s="1" t="n"/>
       <c r="O1" s="1" t="n"/>
       <c r="P1" s="1" t="n"/>
@@ -493,223 +493,435 @@
       <c r="U1" s="1" t="n"/>
       <c r="V1" s="1" t="n"/>
       <c r="W1" s="1" t="n"/>
+      <c r="X1" s="1" t="n"/>
+      <c r="Y1" s="1" t="n"/>
+      <c r="Z1" s="1" t="n"/>
+      <c r="AA1" s="1" t="n"/>
+      <c r="AB1" s="1" t="n"/>
+      <c r="AC1" s="1" t="n"/>
+      <c r="AD1" s="1" t="n"/>
+      <c r="AE1" s="1" t="n"/>
+      <c r="AF1" s="1" t="n"/>
+      <c r="AG1" s="1" t="n"/>
+      <c r="AH1" s="1" t="n"/>
+      <c r="AI1" s="1" t="n"/>
+      <c r="AJ1" s="1" t="n"/>
+      <c r="AK1" s="1" t="n"/>
+      <c r="AL1" s="1" t="n"/>
+      <c r="AM1" s="1" t="n"/>
+      <c r="AN1" s="1" t="n"/>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="n"/>
+      <c r="AQ1" s="1" t="n"/>
+      <c r="AR1" s="1" t="n"/>
+      <c r="AS1" s="1" t="n"/>
+      <c r="AT1" s="1" t="n"/>
+      <c r="AU1" s="1" t="n"/>
+      <c r="AV1" s="1" t="n"/>
+      <c r="AW1" s="1" t="n"/>
+      <c r="AX1" s="1" t="n"/>
+      <c r="AY1" s="1" t="n"/>
+      <c r="AZ1" s="1" t="n"/>
+      <c r="BA1" s="1" t="n"/>
+      <c r="BB1" s="1" t="n"/>
+      <c r="BC1" s="1" t="n"/>
+      <c r="BD1" s="1" t="n"/>
+      <c r="BE1" s="1" t="n"/>
+      <c r="BF1" s="1" t="n"/>
+      <c r="BG1" s="1" t="n"/>
+      <c r="BH1" s="1" t="n"/>
+      <c r="BI1" s="1" t="n"/>
+      <c r="BJ1" s="1" t="n"/>
+      <c r="BK1" s="1" t="n"/>
+      <c r="BL1" s="1" t="n"/>
+      <c r="BM1" s="1" t="n"/>
+      <c r="BN1" s="1" t="n"/>
+      <c r="BO1" s="1" t="n"/>
+      <c r="BP1" s="1" t="n"/>
+      <c r="BQ1" s="1" t="n"/>
+      <c r="BR1" s="1" t="n"/>
+      <c r="BS1" s="1" t="n"/>
+      <c r="BT1" s="1" t="n"/>
+      <c r="BU1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Color</t>
+          <t>Correct</t>
         </is>
       </c>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="n"/>
-      <c r="E2" s="1" t="n"/>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Borderline</t>
+        </is>
+      </c>
       <c r="F2" s="1" t="n"/>
       <c r="G2" s="1" t="n"/>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Color</t>
         </is>
       </c>
       <c r="I2" s="1" t="n"/>
       <c r="J2" s="1" t="n"/>
       <c r="K2" s="1" t="n"/>
-      <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>Area</t>
-        </is>
-      </c>
-      <c r="M2" s="1" t="inlineStr">
-        <is>
-          <t>Color</t>
-        </is>
-      </c>
+      <c r="L2" s="1" t="n"/>
+      <c r="M2" s="1" t="n"/>
       <c r="N2" s="1" t="n"/>
       <c r="O2" s="1" t="n"/>
       <c r="P2" s="1" t="n"/>
       <c r="Q2" s="1" t="n"/>
       <c r="R2" s="1" t="n"/>
-      <c r="S2" s="1" t="inlineStr">
-        <is>
-          <t>Location</t>
-        </is>
-      </c>
+      <c r="S2" s="1" t="n"/>
       <c r="T2" s="1" t="n"/>
       <c r="U2" s="1" t="n"/>
       <c r="V2" s="1" t="n"/>
-      <c r="W2" s="1" t="inlineStr">
+      <c r="W2" s="1" t="n"/>
+      <c r="X2" s="1" t="n"/>
+      <c r="Y2" s="1" t="n"/>
+      <c r="Z2" s="1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="AA2" s="1" t="n"/>
+      <c r="AB2" s="1" t="n"/>
+      <c r="AC2" s="1" t="n"/>
+      <c r="AD2" s="1" t="n"/>
+      <c r="AE2" s="1" t="n"/>
+      <c r="AF2" s="1" t="n"/>
+      <c r="AG2" s="1" t="n"/>
+      <c r="AH2" s="1" t="n"/>
+      <c r="AI2" s="1" t="n"/>
+      <c r="AJ2" s="1" t="n"/>
+      <c r="AK2" s="1" t="n"/>
+      <c r="AL2" s="1" t="inlineStr">
         <is>
           <t>Area</t>
         </is>
       </c>
+      <c r="AM2" s="1" t="n"/>
+      <c r="AN2" s="1" t="n"/>
+      <c r="AO2" s="1" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="AP2" s="1" t="n"/>
+      <c r="AQ2" s="1" t="n"/>
+      <c r="AR2" s="1" t="n"/>
+      <c r="AS2" s="1" t="n"/>
+      <c r="AT2" s="1" t="n"/>
+      <c r="AU2" s="1" t="n"/>
+      <c r="AV2" s="1" t="n"/>
+      <c r="AW2" s="1" t="n"/>
+      <c r="AX2" s="1" t="n"/>
+      <c r="AY2" s="1" t="n"/>
+      <c r="AZ2" s="1" t="n"/>
+      <c r="BA2" s="1" t="n"/>
+      <c r="BB2" s="1" t="n"/>
+      <c r="BC2" s="1" t="n"/>
+      <c r="BD2" s="1" t="n"/>
+      <c r="BE2" s="1" t="n"/>
+      <c r="BF2" s="1" t="n"/>
+      <c r="BG2" s="1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="BH2" s="1" t="n"/>
+      <c r="BI2" s="1" t="n"/>
+      <c r="BJ2" s="1" t="n"/>
+      <c r="BK2" s="1" t="n"/>
+      <c r="BL2" s="1" t="n"/>
+      <c r="BM2" s="1" t="n"/>
+      <c r="BN2" s="1" t="n"/>
+      <c r="BO2" s="1" t="n"/>
+      <c r="BP2" s="1" t="n"/>
+      <c r="BQ2" s="1" t="n"/>
+      <c r="BR2" s="1" t="n"/>
+      <c r="BS2" s="1" t="inlineStr">
+        <is>
+          <t>Area</t>
+        </is>
+      </c>
+      <c r="BT2" s="1" t="n"/>
+      <c r="BU2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr"/>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>Center</t>
-        </is>
-      </c>
+      <c r="B3" s="1" t="inlineStr"/>
       <c r="C3" s="1" t="n"/>
       <c r="D3" s="1" t="n"/>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>Range</t>
-        </is>
-      </c>
+      <c r="E3" s="1" t="inlineStr"/>
       <c r="F3" s="1" t="n"/>
       <c r="G3" s="1" t="n"/>
       <c r="H3" s="1" t="inlineStr">
         <is>
-          <t>Mean</t>
+          <t>Center</t>
         </is>
       </c>
       <c r="I3" s="1" t="n"/>
-      <c r="J3" s="1" t="inlineStr">
-        <is>
-          <t>SD</t>
-        </is>
-      </c>
+      <c r="J3" s="1" t="n"/>
       <c r="K3" s="1" t="n"/>
-      <c r="L3" s="1" t="inlineStr"/>
-      <c r="M3" s="1" t="inlineStr">
-        <is>
-          <t>Center</t>
-        </is>
-      </c>
+      <c r="L3" s="1" t="n"/>
+      <c r="M3" s="1" t="n"/>
       <c r="N3" s="1" t="n"/>
       <c r="O3" s="1" t="n"/>
-      <c r="P3" s="1" t="inlineStr">
+      <c r="P3" s="1" t="n"/>
+      <c r="Q3" s="1" t="inlineStr">
         <is>
           <t>Range</t>
         </is>
       </c>
-      <c r="Q3" s="1" t="n"/>
       <c r="R3" s="1" t="n"/>
-      <c r="S3" s="1" t="inlineStr">
+      <c r="S3" s="1" t="n"/>
+      <c r="T3" s="1" t="n"/>
+      <c r="U3" s="1" t="n"/>
+      <c r="V3" s="1" t="n"/>
+      <c r="W3" s="1" t="n"/>
+      <c r="X3" s="1" t="n"/>
+      <c r="Y3" s="1" t="n"/>
+      <c r="Z3" s="1" t="inlineStr">
         <is>
           <t>Mean</t>
         </is>
       </c>
-      <c r="T3" s="1" t="n"/>
-      <c r="U3" s="1" t="inlineStr">
+      <c r="AA3" s="1" t="n"/>
+      <c r="AB3" s="1" t="n"/>
+      <c r="AC3" s="1" t="n"/>
+      <c r="AD3" s="1" t="n"/>
+      <c r="AE3" s="1" t="n"/>
+      <c r="AF3" s="1" t="inlineStr">
         <is>
           <t>SD</t>
         </is>
       </c>
-      <c r="V3" s="1" t="n"/>
-      <c r="W3" s="1" t="inlineStr"/>
+      <c r="AG3" s="1" t="n"/>
+      <c r="AH3" s="1" t="n"/>
+      <c r="AI3" s="1" t="n"/>
+      <c r="AJ3" s="1" t="n"/>
+      <c r="AK3" s="1" t="n"/>
+      <c r="AL3" s="1" t="inlineStr"/>
+      <c r="AM3" s="1" t="n"/>
+      <c r="AN3" s="1" t="n"/>
+      <c r="AO3" s="1" t="inlineStr">
+        <is>
+          <t>Center</t>
+        </is>
+      </c>
+      <c r="AP3" s="1" t="n"/>
+      <c r="AQ3" s="1" t="n"/>
+      <c r="AR3" s="1" t="n"/>
+      <c r="AS3" s="1" t="n"/>
+      <c r="AT3" s="1" t="n"/>
+      <c r="AU3" s="1" t="n"/>
+      <c r="AV3" s="1" t="n"/>
+      <c r="AW3" s="1" t="n"/>
+      <c r="AX3" s="1" t="inlineStr">
+        <is>
+          <t>Range</t>
+        </is>
+      </c>
+      <c r="AY3" s="1" t="n"/>
+      <c r="AZ3" s="1" t="n"/>
+      <c r="BA3" s="1" t="n"/>
+      <c r="BB3" s="1" t="n"/>
+      <c r="BC3" s="1" t="n"/>
+      <c r="BD3" s="1" t="n"/>
+      <c r="BE3" s="1" t="n"/>
+      <c r="BF3" s="1" t="n"/>
+      <c r="BG3" s="1" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="BH3" s="1" t="n"/>
+      <c r="BI3" s="1" t="n"/>
+      <c r="BJ3" s="1" t="n"/>
+      <c r="BK3" s="1" t="n"/>
+      <c r="BL3" s="1" t="n"/>
+      <c r="BM3" s="1" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="BN3" s="1" t="n"/>
+      <c r="BO3" s="1" t="n"/>
+      <c r="BP3" s="1" t="n"/>
+      <c r="BQ3" s="1" t="n"/>
+      <c r="BR3" s="1" t="n"/>
+      <c r="BS3" s="1" t="inlineStr"/>
+      <c r="BT3" s="1" t="n"/>
+      <c r="BU3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr"/>
-      <c r="B4" s="1" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
+      <c r="E4" s="1" t="inlineStr"/>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="C4" s="1" t="inlineStr">
+      <c r="I4" s="1" t="n"/>
+      <c r="J4" s="1" t="n"/>
+      <c r="K4" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="D4" s="1" t="inlineStr">
+      <c r="L4" s="1" t="n"/>
+      <c r="M4" s="1" t="n"/>
+      <c r="N4" s="1" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="E4" s="1" t="inlineStr">
+      <c r="O4" s="1" t="n"/>
+      <c r="P4" s="1" t="n"/>
+      <c r="Q4" s="1" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="F4" s="1" t="inlineStr">
+      <c r="R4" s="1" t="n"/>
+      <c r="S4" s="1" t="n"/>
+      <c r="T4" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="G4" s="1" t="inlineStr">
+      <c r="U4" s="1" t="n"/>
+      <c r="V4" s="1" t="n"/>
+      <c r="W4" s="1" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="H4" s="1" t="inlineStr">
+      <c r="X4" s="1" t="n"/>
+      <c r="Y4" s="1" t="n"/>
+      <c r="Z4" s="1" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="I4" s="1" t="inlineStr">
+      <c r="AA4" s="1" t="n"/>
+      <c r="AB4" s="1" t="n"/>
+      <c r="AC4" s="1" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="J4" s="1" t="inlineStr">
+      <c r="AD4" s="1" t="n"/>
+      <c r="AE4" s="1" t="n"/>
+      <c r="AF4" s="1" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="K4" s="1" t="inlineStr">
+      <c r="AG4" s="1" t="n"/>
+      <c r="AH4" s="1" t="n"/>
+      <c r="AI4" s="1" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="L4" s="1" t="inlineStr"/>
-      <c r="M4" s="1" t="inlineStr">
+      <c r="AJ4" s="1" t="n"/>
+      <c r="AK4" s="1" t="n"/>
+      <c r="AL4" s="1" t="inlineStr"/>
+      <c r="AM4" s="1" t="n"/>
+      <c r="AN4" s="1" t="n"/>
+      <c r="AO4" s="1" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="N4" s="1" t="inlineStr">
+      <c r="AP4" s="1" t="n"/>
+      <c r="AQ4" s="1" t="n"/>
+      <c r="AR4" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="O4" s="1" t="inlineStr">
+      <c r="AS4" s="1" t="n"/>
+      <c r="AT4" s="1" t="n"/>
+      <c r="AU4" s="1" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="P4" s="1" t="inlineStr">
+      <c r="AV4" s="1" t="n"/>
+      <c r="AW4" s="1" t="n"/>
+      <c r="AX4" s="1" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="Q4" s="1" t="inlineStr">
+      <c r="AY4" s="1" t="n"/>
+      <c r="AZ4" s="1" t="n"/>
+      <c r="BA4" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="R4" s="1" t="inlineStr">
+      <c r="BB4" s="1" t="n"/>
+      <c r="BC4" s="1" t="n"/>
+      <c r="BD4" s="1" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="S4" s="1" t="inlineStr">
+      <c r="BE4" s="1" t="n"/>
+      <c r="BF4" s="1" t="n"/>
+      <c r="BG4" s="1" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="T4" s="1" t="inlineStr">
+      <c r="BH4" s="1" t="n"/>
+      <c r="BI4" s="1" t="n"/>
+      <c r="BJ4" s="1" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="U4" s="1" t="inlineStr">
+      <c r="BK4" s="1" t="n"/>
+      <c r="BL4" s="1" t="n"/>
+      <c r="BM4" s="1" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="V4" s="1" t="inlineStr">
+      <c r="BN4" s="1" t="n"/>
+      <c r="BO4" s="1" t="n"/>
+      <c r="BP4" s="1" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="W4" s="1" t="inlineStr"/>
+      <c r="BQ4" s="1" t="n"/>
+      <c r="BR4" s="1" t="n"/>
+      <c r="BS4" s="1" t="inlineStr"/>
+      <c r="BT4" s="1" t="n"/>
+      <c r="BU4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>min</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
@@ -719,12 +931,12 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>max</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>min</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
@@ -734,12 +946,12 @@
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>max</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>min</t>
         </is>
       </c>
       <c r="I5" s="1" t="inlineStr">
@@ -749,12 +961,12 @@
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>max</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>min</t>
         </is>
       </c>
       <c r="L5" s="1" t="inlineStr">
@@ -764,12 +976,12 @@
       </c>
       <c r="M5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>max</t>
         </is>
       </c>
       <c r="N5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>min</t>
         </is>
       </c>
       <c r="O5" s="1" t="inlineStr">
@@ -779,12 +991,12 @@
       </c>
       <c r="P5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>max</t>
         </is>
       </c>
       <c r="Q5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>min</t>
         </is>
       </c>
       <c r="R5" s="1" t="inlineStr">
@@ -794,12 +1006,12 @@
       </c>
       <c r="S5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>max</t>
         </is>
       </c>
       <c r="T5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>min</t>
         </is>
       </c>
       <c r="U5" s="1" t="inlineStr">
@@ -809,12 +1021,262 @@
       </c>
       <c r="V5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>max</t>
         </is>
       </c>
       <c r="W5" s="1" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="X5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="Y5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="Z5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="AA5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="AB5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="AC5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="AD5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="AE5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="AF5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="AG5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="AH5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="AI5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="AJ5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="AK5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="AL5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="AM5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="AN5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="AO5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="AP5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="AQ5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="AR5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="AS5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="AT5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="AU5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="AV5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="AW5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="AX5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="AY5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="AZ5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="BA5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="BB5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="BC5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="BD5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="BE5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="BF5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="BG5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="BH5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="BI5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="BJ5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="BK5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="BL5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="BM5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="BN5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="BO5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="BP5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="BQ5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="BR5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="BS5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="BT5" s="1" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="BU5" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
         </is>
       </c>
     </row>
@@ -831,71 +1293,221 @@
           <t>False</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
         <v>6</v>
       </c>
-      <c r="C7" t="n">
+      <c r="J7" t="n">
+        <v>10</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="n">
         <v>6</v>
       </c>
-      <c r="D7" t="n">
+      <c r="M7" t="n">
+        <v>10</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" t="n">
         <v>5</v>
       </c>
-      <c r="E7" t="n">
+      <c r="P7" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>1</v>
+      </c>
+      <c r="R7" t="n">
         <v>6</v>
       </c>
-      <c r="F7" t="n">
+      <c r="S7" t="n">
+        <v>10</v>
+      </c>
+      <c r="T7" t="n">
+        <v>1</v>
+      </c>
+      <c r="U7" t="n">
         <v>5</v>
       </c>
-      <c r="G7" t="n">
+      <c r="V7" t="n">
+        <v>10</v>
+      </c>
+      <c r="W7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X7" t="n">
         <v>6</v>
       </c>
-      <c r="H7" t="n">
+      <c r="Y7" t="n">
+        <v>10</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA7" t="n">
         <v>6</v>
       </c>
-      <c r="I7" t="n">
+      <c r="AB7" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD7" t="n">
         <v>5</v>
       </c>
-      <c r="J7" t="n">
+      <c r="AE7" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG7" t="n">
         <v>5</v>
       </c>
-      <c r="K7" t="n">
+      <c r="AH7" t="n">
+        <v>10</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ7" t="n">
         <v>5</v>
       </c>
-      <c r="L7" t="n">
+      <c r="AK7" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM7" t="n">
         <v>5</v>
       </c>
-      <c r="M7" t="n">
+      <c r="AN7" t="n">
+        <v>10</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP7" t="n">
         <v>112</v>
       </c>
-      <c r="N7" t="n">
-        <v>99</v>
-      </c>
-      <c r="O7" t="n">
-        <v>95</v>
-      </c>
-      <c r="P7" t="n">
-        <v>74</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>111</v>
-      </c>
-      <c r="R7" t="n">
-        <v>116</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0.4918166415411495</v>
-      </c>
-      <c r="T7" t="n">
-        <v>0.3776903920920894</v>
-      </c>
-      <c r="U7" t="n">
-        <v>0.1631553513124193</v>
-      </c>
-      <c r="V7" t="n">
-        <v>0.1528619334065977</v>
-      </c>
-      <c r="W7" t="n">
-        <v>0.06255933168786786</v>
+      <c r="AQ7" t="n">
+        <v>171</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>96</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>255</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>96</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>240</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>76</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>255</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>115</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>254</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>115</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>249</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>0.1917208752217622</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>0.4924638246619958</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>0.7971996797990597</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>0.1267264845246497</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>0.3800195886385897</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>0.8576273189176415</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN7" t="n">
+        <v>0.1616921241529301</v>
+      </c>
+      <c r="BO7" t="n">
+        <v>0.3815918678883275</v>
+      </c>
+      <c r="BP7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ7" t="n">
+        <v>0.1531954201457461</v>
+      </c>
+      <c r="BR7" t="n">
+        <v>0.4084038538883136</v>
+      </c>
+      <c r="BS7" t="n">
+        <v>4.528985507246377e-05</v>
+      </c>
+      <c r="BT7" t="n">
+        <v>0.06068775633120142</v>
+      </c>
+      <c r="BU7" t="n">
+        <v>0.4788255223037832</v>
       </c>
     </row>
     <row r="8">
@@ -904,71 +1516,221 @@
           <t>Maybe</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
         <v>4</v>
       </c>
-      <c r="C8" t="n">
-        <v>5</v>
-      </c>
-      <c r="D8" t="n">
-        <v>6</v>
-      </c>
-      <c r="E8" t="n">
-        <v>5</v>
-      </c>
-      <c r="F8" t="n">
-        <v>6</v>
-      </c>
-      <c r="G8" t="n">
-        <v>4</v>
-      </c>
-      <c r="H8" t="n">
-        <v>4</v>
-      </c>
-      <c r="I8" t="n">
-        <v>6</v>
-      </c>
       <c r="J8" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K8" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
         <v>5</v>
       </c>
       <c r="M8" t="n">
-        <v>111</v>
+        <v>10</v>
       </c>
       <c r="N8" t="n">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="O8" t="n">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="P8" t="n">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="Q8" t="n">
-        <v>129</v>
+        <v>1</v>
       </c>
       <c r="R8" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="S8" t="n">
-        <v>0.4811666571007671</v>
+        <v>10</v>
       </c>
       <c r="T8" t="n">
-        <v>0.4011653397946234</v>
+        <v>1</v>
       </c>
       <c r="U8" t="n">
-        <v>0.2086074387397381</v>
+        <v>6</v>
       </c>
       <c r="V8" t="n">
-        <v>0.2078646580837262</v>
+        <v>10</v>
       </c>
       <c r="W8" t="n">
-        <v>0.08036016846589533</v>
+        <v>1</v>
+      </c>
+      <c r="X8" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>6</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>6</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>7</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>110</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>121</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>9</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>91</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>142</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>87</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>132</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>204</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>30</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>72</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>186</v>
+      </c>
+      <c r="BA8" t="n">
+        <v>26</v>
+      </c>
+      <c r="BB8" t="n">
+        <v>125</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>195</v>
+      </c>
+      <c r="BD8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE8" t="n">
+        <v>65</v>
+      </c>
+      <c r="BF8" t="n">
+        <v>158</v>
+      </c>
+      <c r="BG8" t="n">
+        <v>0.2971202980704722</v>
+      </c>
+      <c r="BH8" t="n">
+        <v>0.4750289094045609</v>
+      </c>
+      <c r="BI8" t="n">
+        <v>0.6436457022313037</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>0.2521664153312215</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>0.4816744520301833</v>
+      </c>
+      <c r="BL8" t="n">
+        <v>0.7930299494360175</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>0.0183147377542188</v>
+      </c>
+      <c r="BN8" t="n">
+        <v>0.2540160981830425</v>
+      </c>
+      <c r="BO8" t="n">
+        <v>0.3621832297737324</v>
+      </c>
+      <c r="BP8" t="n">
+        <v>0.02383851167434846</v>
+      </c>
+      <c r="BQ8" t="n">
+        <v>0.2293859161181213</v>
+      </c>
+      <c r="BR8" t="n">
+        <v>0.371993319670845</v>
+      </c>
+      <c r="BS8" t="n">
+        <v>0.002197802197802198</v>
+      </c>
+      <c r="BT8" t="n">
+        <v>0.09444740281744687</v>
+      </c>
+      <c r="BU8" t="n">
+        <v>0.3924858223062382</v>
       </c>
     </row>
     <row r="9">
@@ -977,89 +1739,272 @@
           <t>True</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
         <v>4</v>
       </c>
-      <c r="C9" t="n">
+      <c r="J9" t="n">
+        <v>10</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" t="n">
         <v>4</v>
       </c>
-      <c r="D9" t="n">
+      <c r="M9" t="n">
+        <v>10</v>
+      </c>
+      <c r="N9" t="n">
+        <v>4</v>
+      </c>
+      <c r="O9" t="n">
         <v>9</v>
       </c>
-      <c r="E9" t="n">
+      <c r="P9" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" t="n">
         <v>5</v>
       </c>
-      <c r="F9" t="n">
+      <c r="S9" t="n">
+        <v>10</v>
+      </c>
+      <c r="T9" t="n">
+        <v>1</v>
+      </c>
+      <c r="U9" t="n">
         <v>8</v>
       </c>
-      <c r="G9" t="n">
-        <v>3</v>
-      </c>
-      <c r="H9" t="n">
-        <v>5</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="V9" t="n">
+        <v>10</v>
+      </c>
+      <c r="W9" t="n">
+        <v>1</v>
+      </c>
+      <c r="X9" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>7</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD9" t="n">
         <v>8</v>
       </c>
-      <c r="J9" t="n">
+      <c r="AE9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ9" t="n">
         <v>7</v>
       </c>
-      <c r="K9" t="n">
+      <c r="AK9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM9" t="n">
         <v>7</v>
       </c>
-      <c r="L9" t="n">
-        <v>7</v>
-      </c>
-      <c r="M9" t="n">
+      <c r="AN9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP9" t="n">
         <v>111</v>
       </c>
-      <c r="N9" t="n">
-        <v>55</v>
-      </c>
-      <c r="O9" t="n">
-        <v>172</v>
-      </c>
-      <c r="P9" t="n">
-        <v>74</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>147.5</v>
-      </c>
-      <c r="R9" t="n">
-        <v>38</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0.4833145618205442</v>
-      </c>
-      <c r="T9" t="n">
-        <v>0.482209015300243</v>
-      </c>
-      <c r="U9" t="n">
-        <v>0.1788085118116693</v>
-      </c>
-      <c r="V9" t="n">
-        <v>0.156555073083308</v>
-      </c>
-      <c r="W9" t="n">
-        <v>0.06783159117938689</v>
+      <c r="AQ9" t="n">
+        <v>173</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>54</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>161</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>83</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>173.5</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>253</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>8</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>73</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>251</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>26</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>147</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>247</v>
+      </c>
+      <c r="BD9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE9" t="n">
+        <v>34</v>
+      </c>
+      <c r="BF9" t="n">
+        <v>145</v>
+      </c>
+      <c r="BG9" t="n">
+        <v>0.2926452366370901</v>
+      </c>
+      <c r="BH9" t="n">
+        <v>0.4716005963708375</v>
+      </c>
+      <c r="BI9" t="n">
+        <v>0.7314275151930459</v>
+      </c>
+      <c r="BJ9" t="n">
+        <v>0.2781909373919059</v>
+      </c>
+      <c r="BK9" t="n">
+        <v>0.4869602453773775</v>
+      </c>
+      <c r="BL9" t="n">
+        <v>0.8265421102335169</v>
+      </c>
+      <c r="BM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN9" t="n">
+        <v>0.1859438422254086</v>
+      </c>
+      <c r="BO9" t="n">
+        <v>0.3799202326208149</v>
+      </c>
+      <c r="BP9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ9" t="n">
+        <v>0.1626646947964439</v>
+      </c>
+      <c r="BR9" t="n">
+        <v>0.3927689016038371</v>
+      </c>
+      <c r="BS9" t="n">
+        <v>5.947071067499257e-05</v>
+      </c>
+      <c r="BT9" t="n">
+        <v>0.06926673148846588</v>
+      </c>
+      <c r="BU9" t="n">
+        <v>0.417966903073286</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="M2:R2"/>
-    <mergeCell ref="S2:V2"/>
+  <mergeCells count="47">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:AN1"/>
+    <mergeCell ref="AO1:BU1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:Y2"/>
+    <mergeCell ref="Z2:AK2"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AO2:BF2"/>
+    <mergeCell ref="BG2:BR2"/>
+    <mergeCell ref="BS2:BU2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="Q3:Y3"/>
+    <mergeCell ref="Z3:AE3"/>
+    <mergeCell ref="AF3:AK3"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="AO3:AW3"/>
+    <mergeCell ref="AX3:BF3"/>
+    <mergeCell ref="BG3:BL3"/>
+    <mergeCell ref="BM3:BR3"/>
+    <mergeCell ref="BS3:BU3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="W4:Y4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="AL4:AN4"/>
+    <mergeCell ref="AO4:AQ4"/>
+    <mergeCell ref="AR4:AT4"/>
+    <mergeCell ref="AU4:AW4"/>
+    <mergeCell ref="AX4:AZ4"/>
+    <mergeCell ref="BA4:BC4"/>
+    <mergeCell ref="BD4:BF4"/>
+    <mergeCell ref="BG4:BI4"/>
+    <mergeCell ref="BJ4:BL4"/>
+    <mergeCell ref="BM4:BO4"/>
+    <mergeCell ref="BP4:BR4"/>
+    <mergeCell ref="BS4:BU4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Committing new kmeans clusters data and outputs
</commit_message>
<xml_diff>
--- a/data/03_first_25percent_metrics/color_and_spatial_metrics_agg.xlsx
+++ b/data/03_first_25percent_metrics/color_and_spatial_metrics_agg.xlsx
@@ -1315,7 +1315,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J7" t="n">
         <v>10</v>
@@ -1324,7 +1324,7 @@
         <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M7" t="n">
         <v>10</v>
@@ -1360,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="X7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y7" t="n">
         <v>10</v>
@@ -1414,100 +1414,100 @@
         <v>0</v>
       </c>
       <c r="AP7" t="n">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="AQ7" t="n">
-        <v>173</v>
+        <v>249</v>
       </c>
       <c r="AR7" t="n">
         <v>0</v>
       </c>
       <c r="AS7" t="n">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="AT7" t="n">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="AU7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV7" t="n">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="AW7" t="n">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="AX7" t="n">
         <v>0</v>
       </c>
       <c r="AY7" t="n">
-        <v>75.5</v>
+        <v>52.5</v>
       </c>
       <c r="AZ7" t="n">
-        <v>255</v>
+        <v>227</v>
       </c>
       <c r="BA7" t="n">
         <v>0</v>
       </c>
       <c r="BB7" t="n">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="BC7" t="n">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="BD7" t="n">
         <v>0</v>
       </c>
       <c r="BE7" t="n">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="BF7" t="n">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="BG7" t="n">
-        <v>0.1917208752217622</v>
+        <v>0.2199918496694308</v>
       </c>
       <c r="BH7" t="n">
-        <v>0.4923741665533928</v>
+        <v>0.4840675790259474</v>
       </c>
       <c r="BI7" t="n">
-        <v>0.792275890580858</v>
+        <v>0.7584608065647381</v>
       </c>
       <c r="BJ7" t="n">
-        <v>0.1267264845246497</v>
+        <v>0.1595579165732227</v>
       </c>
       <c r="BK7" t="n">
-        <v>0.3794919648207364</v>
+        <v>0.3620032855624651</v>
       </c>
       <c r="BL7" t="n">
-        <v>0.8130156118933797</v>
+        <v>0.8168302750401147</v>
       </c>
       <c r="BM7" t="n">
         <v>0</v>
       </c>
       <c r="BN7" t="n">
-        <v>0.1636675862711519</v>
+        <v>0.1297171271880406</v>
       </c>
       <c r="BO7" t="n">
-        <v>0.3815918678883275</v>
+        <v>0.3715187419335101</v>
       </c>
       <c r="BP7" t="n">
         <v>0</v>
       </c>
       <c r="BQ7" t="n">
-        <v>0.1566647428965612</v>
+        <v>0.1393776221114097</v>
       </c>
       <c r="BR7" t="n">
-        <v>0.3786705113095653</v>
+        <v>0.3857636096137051</v>
       </c>
       <c r="BS7" t="n">
         <v>4.528985507246377e-05</v>
       </c>
       <c r="BT7" t="n">
-        <v>0.06240352517572566</v>
+        <v>0.056342058562631</v>
       </c>
       <c r="BU7" t="n">
-        <v>0.4788255223037832</v>
+        <v>0.5379227053140097</v>
       </c>
     </row>
     <row r="8">
@@ -1550,7 +1550,7 @@
         <v>6</v>
       </c>
       <c r="M8" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N8" t="n">
         <v>3</v>
@@ -1565,16 +1565,16 @@
         <v>1</v>
       </c>
       <c r="R8" t="n">
+        <v>5</v>
+      </c>
+      <c r="S8" t="n">
+        <v>10</v>
+      </c>
+      <c r="T8" t="n">
+        <v>1</v>
+      </c>
+      <c r="U8" t="n">
         <v>6</v>
-      </c>
-      <c r="S8" t="n">
-        <v>10</v>
-      </c>
-      <c r="T8" t="n">
-        <v>2</v>
-      </c>
-      <c r="U8" t="n">
-        <v>7</v>
       </c>
       <c r="V8" t="n">
         <v>10</v>
@@ -1586,7 +1586,7 @@
         <v>5</v>
       </c>
       <c r="Y8" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Z8" t="n">
         <v>1</v>
@@ -1598,7 +1598,7 @@
         <v>10</v>
       </c>
       <c r="AC8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD8" t="n">
         <v>6</v>
@@ -1622,7 +1622,7 @@
         <v>5</v>
       </c>
       <c r="AK8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AL8" t="n">
         <v>1</v>
@@ -1631,106 +1631,106 @@
         <v>5</v>
       </c>
       <c r="AN8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AO8" t="n">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="AP8" t="n">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="AQ8" t="n">
-        <v>171</v>
+        <v>216</v>
       </c>
       <c r="AR8" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="AS8" t="n">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="AT8" t="n">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="AU8" t="n">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="AV8" t="n">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="AW8" t="n">
         <v>224</v>
       </c>
       <c r="AX8" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="AY8" t="n">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="AZ8" t="n">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="BA8" t="n">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="BB8" t="n">
-        <v>121</v>
+        <v>75</v>
       </c>
       <c r="BC8" t="n">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="BD8" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="BE8" t="n">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="BF8" t="n">
-        <v>201</v>
+        <v>166</v>
       </c>
       <c r="BG8" t="n">
-        <v>0.2431331271123332</v>
+        <v>0.3674393175967152</v>
       </c>
       <c r="BH8" t="n">
-        <v>0.4866983734881781</v>
+        <v>0.5081554580896692</v>
       </c>
       <c r="BI8" t="n">
-        <v>0.6440012630324337</v>
+        <v>0.6702758497203591</v>
       </c>
       <c r="BJ8" t="n">
-        <v>0.2422707206184887</v>
+        <v>0.266748786860769</v>
       </c>
       <c r="BK8" t="n">
-        <v>0.4110188152969098</v>
+        <v>0.4241891200148915</v>
       </c>
       <c r="BL8" t="n">
-        <v>0.760374744342548</v>
+        <v>0.8362416904083571</v>
       </c>
       <c r="BM8" t="n">
-        <v>0.01001946183559667</v>
+        <v>0.008546429221175591</v>
       </c>
       <c r="BN8" t="n">
-        <v>0.2152693621383455</v>
+        <v>0.2361582005224207</v>
       </c>
       <c r="BO8" t="n">
-        <v>0.3575142136658729</v>
+        <v>0.3353329333524587</v>
       </c>
       <c r="BP8" t="n">
-        <v>0.02403318448967668</v>
+        <v>0.02056887902668939</v>
       </c>
       <c r="BQ8" t="n">
-        <v>0.1783599280155433</v>
+        <v>0.1614934391458424</v>
       </c>
       <c r="BR8" t="n">
-        <v>0.3623460823462856</v>
+        <v>0.3300403890540208</v>
       </c>
       <c r="BS8" t="n">
-        <v>0.002873012832790653</v>
+        <v>0.001008064516129032</v>
       </c>
       <c r="BT8" t="n">
-        <v>0.06817097605190345</v>
+        <v>0.08737958077165126</v>
       </c>
       <c r="BU8" t="n">
-        <v>0.3319775596072931</v>
+        <v>0.3682476943346509</v>
       </c>
     </row>
     <row r="9">
@@ -1758,19 +1758,19 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I9" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J9" t="n">
         <v>10</v>
       </c>
       <c r="K9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L9" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M9" t="n">
         <v>10</v>
@@ -1788,44 +1788,44 @@
         <v>1</v>
       </c>
       <c r="R9" t="n">
+        <v>7</v>
+      </c>
+      <c r="S9" t="n">
+        <v>10</v>
+      </c>
+      <c r="T9" t="n">
+        <v>1</v>
+      </c>
+      <c r="U9" t="n">
+        <v>8</v>
+      </c>
+      <c r="V9" t="n">
+        <v>10</v>
+      </c>
+      <c r="W9" t="n">
+        <v>1</v>
+      </c>
+      <c r="X9" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>10</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA9" t="n">
         <v>6</v>
       </c>
-      <c r="S9" t="n">
-        <v>10</v>
-      </c>
-      <c r="T9" t="n">
-        <v>1</v>
-      </c>
-      <c r="U9" t="n">
+      <c r="AB9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD9" t="n">
         <v>7</v>
       </c>
-      <c r="V9" t="n">
-        <v>10</v>
-      </c>
-      <c r="W9" t="n">
-        <v>1</v>
-      </c>
-      <c r="X9" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>9</v>
-      </c>
-      <c r="Z9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA9" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB9" t="n">
-        <v>10</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>8</v>
-      </c>
       <c r="AE9" t="n">
         <v>10</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="AG9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AH9" t="n">
         <v>10</v>
@@ -1842,7 +1842,7 @@
         <v>1</v>
       </c>
       <c r="AJ9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AK9" t="n">
         <v>10</v>
@@ -1851,109 +1851,109 @@
         <v>1</v>
       </c>
       <c r="AM9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AN9" t="n">
         <v>10</v>
       </c>
       <c r="AO9" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AP9" t="n">
-        <v>111</v>
+        <v>174</v>
       </c>
       <c r="AQ9" t="n">
-        <v>157</v>
+        <v>247</v>
       </c>
       <c r="AR9" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="AS9" t="n">
-        <v>54</v>
+        <v>145</v>
       </c>
       <c r="AT9" t="n">
-        <v>170</v>
+        <v>246</v>
       </c>
       <c r="AU9" t="n">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="AV9" t="n">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="AW9" t="n">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="AX9" t="n">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="AY9" t="n">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="AZ9" t="n">
+        <v>254</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>13</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>88</v>
+      </c>
+      <c r="BC9" t="n">
         <v>255</v>
       </c>
-      <c r="BA9" t="n">
-        <v>14</v>
-      </c>
-      <c r="BB9" t="n">
-        <v>150</v>
-      </c>
-      <c r="BC9" t="n">
-        <v>254</v>
-      </c>
       <c r="BD9" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BE9" t="n">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="BF9" t="n">
-        <v>174</v>
+        <v>250</v>
       </c>
       <c r="BG9" t="n">
-        <v>0.2855836114350042</v>
+        <v>0.2767811898246681</v>
       </c>
       <c r="BH9" t="n">
-        <v>0.4776131197979734</v>
+        <v>0.4856298763940123</v>
       </c>
       <c r="BI9" t="n">
-        <v>0.7971996797990597</v>
+        <v>0.7780041535708658</v>
       </c>
       <c r="BJ9" t="n">
-        <v>0.2244793776157688</v>
+        <v>0.2414814814814815</v>
       </c>
       <c r="BK9" t="n">
-        <v>0.4877667984189723</v>
+        <v>0.4562394127611517</v>
       </c>
       <c r="BL9" t="n">
-        <v>0.8576273189176415</v>
+        <v>0.8539388543338676</v>
       </c>
       <c r="BM9" t="n">
-        <v>0.007876321702510104</v>
+        <v>0.00206756368767997</v>
       </c>
       <c r="BN9" t="n">
-        <v>0.1812784857191828</v>
+        <v>0.182918138489462</v>
       </c>
       <c r="BO9" t="n">
-        <v>0.3799202326208149</v>
+        <v>0.35608683236975</v>
       </c>
       <c r="BP9" t="n">
-        <v>0.009974597124807026</v>
+        <v>0.005068865814957325</v>
       </c>
       <c r="BQ9" t="n">
-        <v>0.1446111831889948</v>
+        <v>0.1529829903340158</v>
       </c>
       <c r="BR9" t="n">
-        <v>0.4084038538883136</v>
+        <v>0.3487574031177041</v>
       </c>
       <c r="BS9" t="n">
-        <v>0.0008960573476702509</v>
+        <v>0.000139366347672582</v>
       </c>
       <c r="BT9" t="n">
-        <v>0.06143162393162393</v>
+        <v>0.04840579710144927</v>
       </c>
       <c r="BU9" t="n">
-        <v>0.3924858223062382</v>
+        <v>0.4774866569626395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated label values & reran plots
</commit_message>
<xml_diff>
--- a/data/03_first_25percent_metrics/color_and_spatial_metrics_agg.xlsx
+++ b/data/03_first_25percent_metrics/color_and_spatial_metrics_agg.xlsx
@@ -1315,142 +1315,142 @@
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J7" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="K7" t="n">
         <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M7" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="N7" t="n">
         <v>1</v>
       </c>
       <c r="O7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P7" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="Q7" t="n">
         <v>1</v>
       </c>
       <c r="R7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S7" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="T7" t="n">
         <v>1</v>
       </c>
       <c r="U7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="V7" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="W7" t="n">
         <v>1</v>
       </c>
       <c r="X7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Y7" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="Z7" t="n">
         <v>1</v>
       </c>
       <c r="AA7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AB7" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="AC7" t="n">
         <v>1</v>
       </c>
       <c r="AD7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AE7" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="AF7" t="n">
         <v>1</v>
       </c>
       <c r="AG7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AH7" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="AI7" t="n">
         <v>1</v>
       </c>
       <c r="AJ7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AK7" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AL7" t="n">
         <v>1</v>
       </c>
       <c r="AM7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AN7" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AO7" t="n">
         <v>0</v>
       </c>
       <c r="AP7" t="n">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="AQ7" t="n">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="AR7" t="n">
         <v>0</v>
       </c>
       <c r="AS7" t="n">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="AT7" t="n">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="AU7" t="n">
         <v>0</v>
       </c>
       <c r="AV7" t="n">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="AW7" t="n">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="AX7" t="n">
         <v>0</v>
       </c>
       <c r="AY7" t="n">
-        <v>52.5</v>
+        <v>65</v>
       </c>
       <c r="AZ7" t="n">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="BA7" t="n">
         <v>0</v>
       </c>
       <c r="BB7" t="n">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="BC7" t="n">
         <v>230</v>
@@ -1459,55 +1459,55 @@
         <v>0</v>
       </c>
       <c r="BE7" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="BF7" t="n">
         <v>228</v>
       </c>
       <c r="BG7" t="n">
-        <v>0.2199918496694308</v>
+        <v>0.2431951060327109</v>
       </c>
       <c r="BH7" t="n">
-        <v>0.4840675790259474</v>
+        <v>0.5016769669062087</v>
       </c>
       <c r="BI7" t="n">
-        <v>0.7584608065647381</v>
+        <v>1</v>
       </c>
       <c r="BJ7" t="n">
-        <v>0.1595579165732227</v>
+        <v>0</v>
       </c>
       <c r="BK7" t="n">
-        <v>0.3620032855624651</v>
+        <v>0.406294602583436</v>
       </c>
       <c r="BL7" t="n">
-        <v>0.8168302750401147</v>
+        <v>0.9929078014184397</v>
       </c>
       <c r="BM7" t="n">
         <v>0</v>
       </c>
       <c r="BN7" t="n">
-        <v>0.1297171271880406</v>
+        <v>0.1497718489638923</v>
       </c>
       <c r="BO7" t="n">
-        <v>0.3715187419335101</v>
+        <v>0.3938661711008237</v>
       </c>
       <c r="BP7" t="n">
         <v>0</v>
       </c>
       <c r="BQ7" t="n">
-        <v>0.1393776221114097</v>
+        <v>0.1542546444780535</v>
       </c>
       <c r="BR7" t="n">
-        <v>0.3857636096137051</v>
+        <v>0.4435346124233666</v>
       </c>
       <c r="BS7" t="n">
-        <v>4.528985507246377e-05</v>
+        <v>4.585473220836391e-05</v>
       </c>
       <c r="BT7" t="n">
-        <v>0.056342058562631</v>
+        <v>0.04866770861981455</v>
       </c>
       <c r="BU7" t="n">
-        <v>0.5379227053140097</v>
+        <v>0.5152027027027027</v>
       </c>
     </row>
     <row r="8">
@@ -1523,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -1538,7 +1538,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="J8" t="n">
         <v>10</v>
@@ -1553,184 +1553,184 @@
         <v>10</v>
       </c>
       <c r="N8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O8" t="n">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="P8" t="n">
         <v>10</v>
       </c>
       <c r="Q8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" t="n">
         <v>5</v>
       </c>
       <c r="S8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U8" t="n">
         <v>6</v>
       </c>
       <c r="V8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="X8" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Y8" t="n">
         <v>10</v>
       </c>
       <c r="Z8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB8" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AC8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>11</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>12</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>6</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>11</v>
+      </c>
+      <c r="AL8" t="n">
         <v>2</v>
       </c>
-      <c r="AD8" t="n">
+      <c r="AM8" t="n">
         <v>6</v>
       </c>
-      <c r="AE8" t="n">
-        <v>10</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG8" t="n">
+      <c r="AN8" t="n">
+        <v>11</v>
+      </c>
+      <c r="AO8" t="n">
         <v>6</v>
       </c>
-      <c r="AH8" t="n">
-        <v>10</v>
-      </c>
-      <c r="AI8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ8" t="n">
-        <v>5</v>
-      </c>
-      <c r="AK8" t="n">
-        <v>9</v>
-      </c>
-      <c r="AL8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM8" t="n">
-        <v>5</v>
-      </c>
-      <c r="AN8" t="n">
-        <v>9</v>
-      </c>
-      <c r="AO8" t="n">
-        <v>41</v>
-      </c>
       <c r="AP8" t="n">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="AQ8" t="n">
-        <v>216</v>
+        <v>179</v>
       </c>
       <c r="AR8" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="AS8" t="n">
-        <v>103</v>
+        <v>75.5</v>
       </c>
       <c r="AT8" t="n">
-        <v>219</v>
+        <v>134</v>
       </c>
       <c r="AU8" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AV8" t="n">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="AW8" t="n">
-        <v>224</v>
+        <v>108</v>
       </c>
       <c r="AX8" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AY8" t="n">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="AZ8" t="n">
-        <v>167</v>
+        <v>95</v>
       </c>
       <c r="BA8" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="BB8" t="n">
-        <v>75</v>
+        <v>44.5</v>
       </c>
       <c r="BC8" t="n">
-        <v>171</v>
+        <v>79</v>
       </c>
       <c r="BD8" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="BE8" t="n">
-        <v>86</v>
+        <v>34.5</v>
       </c>
       <c r="BF8" t="n">
-        <v>166</v>
+        <v>93</v>
       </c>
       <c r="BG8" t="n">
-        <v>0.3674393175967152</v>
+        <v>0.4654117848285294</v>
       </c>
       <c r="BH8" t="n">
-        <v>0.5081554580896692</v>
+        <v>0.5443347513181849</v>
       </c>
       <c r="BI8" t="n">
-        <v>0.6702758497203591</v>
+        <v>0.9870761866773036</v>
       </c>
       <c r="BJ8" t="n">
-        <v>0.266748786860769</v>
+        <v>0.303225806451613</v>
       </c>
       <c r="BK8" t="n">
-        <v>0.4241891200148915</v>
+        <v>0.4294966012707016</v>
       </c>
       <c r="BL8" t="n">
-        <v>0.8362416904083571</v>
+        <v>0.7254102644507164</v>
       </c>
       <c r="BM8" t="n">
-        <v>0.008546429221175591</v>
+        <v>0</v>
       </c>
       <c r="BN8" t="n">
-        <v>0.2361582005224207</v>
+        <v>0.1578496260175382</v>
       </c>
       <c r="BO8" t="n">
-        <v>0.3353329333524587</v>
+        <v>0.3441590921303435</v>
       </c>
       <c r="BP8" t="n">
-        <v>0.02056887902668939</v>
+        <v>0</v>
       </c>
       <c r="BQ8" t="n">
-        <v>0.1614934391458424</v>
+        <v>0.2107149380697658</v>
       </c>
       <c r="BR8" t="n">
-        <v>0.3300403890540208</v>
+        <v>0.3409516951580344</v>
       </c>
       <c r="BS8" t="n">
-        <v>0.001008064516129032</v>
+        <v>2.858286171611502e-05</v>
       </c>
       <c r="BT8" t="n">
-        <v>0.08737958077165126</v>
+        <v>0.04341140999265811</v>
       </c>
       <c r="BU8" t="n">
-        <v>0.3682476943346509</v>
+        <v>0.3021972884525479</v>
       </c>
     </row>
     <row r="9">
@@ -1758,28 +1758,28 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J9" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M9" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P9" t="n">
         <v>10</v>
@@ -1788,28 +1788,28 @@
         <v>1</v>
       </c>
       <c r="R9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S9" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="T9" t="n">
         <v>1</v>
       </c>
       <c r="U9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="V9" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="W9" t="n">
         <v>1</v>
       </c>
       <c r="X9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Y9" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="Z9" t="n">
         <v>1</v>
@@ -1818,16 +1818,16 @@
         <v>6</v>
       </c>
       <c r="AB9" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AC9" t="n">
         <v>1</v>
       </c>
       <c r="AD9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AE9" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="AF9" t="n">
         <v>1</v>
@@ -1836,7 +1836,7 @@
         <v>6</v>
       </c>
       <c r="AH9" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="AI9" t="n">
         <v>1</v>
@@ -1845,7 +1845,7 @@
         <v>6</v>
       </c>
       <c r="AK9" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="AL9" t="n">
         <v>1</v>
@@ -1854,106 +1854,106 @@
         <v>6</v>
       </c>
       <c r="AN9" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="AO9" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="AP9" t="n">
-        <v>174</v>
+        <v>115.5</v>
       </c>
       <c r="AQ9" t="n">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="AR9" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="AS9" t="n">
-        <v>145</v>
+        <v>84</v>
       </c>
       <c r="AT9" t="n">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="AU9" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="AV9" t="n">
-        <v>130</v>
+        <v>70.5</v>
       </c>
       <c r="AW9" t="n">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="AX9" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AY9" t="n">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="AZ9" t="n">
-        <v>254</v>
+        <v>201</v>
       </c>
       <c r="BA9" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="BB9" t="n">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="BC9" t="n">
-        <v>255</v>
+        <v>203</v>
       </c>
       <c r="BD9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="BE9" t="n">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="BF9" t="n">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="BG9" t="n">
-        <v>0.2767811898246681</v>
+        <v>0.2629369803476946</v>
       </c>
       <c r="BH9" t="n">
-        <v>0.4856298763940123</v>
+        <v>0.5079363171785225</v>
       </c>
       <c r="BI9" t="n">
-        <v>0.7780041535708658</v>
+        <v>1</v>
       </c>
       <c r="BJ9" t="n">
-        <v>0.2414814814814815</v>
+        <v>0.1022727272727273</v>
       </c>
       <c r="BK9" t="n">
-        <v>0.4562394127611517</v>
+        <v>0.4255890480611942</v>
       </c>
       <c r="BL9" t="n">
-        <v>0.8539388543338676</v>
+        <v>0.885304659498208</v>
       </c>
       <c r="BM9" t="n">
-        <v>0.00206756368767997</v>
+        <v>0</v>
       </c>
       <c r="BN9" t="n">
-        <v>0.182918138489462</v>
+        <v>0.152633952419462</v>
       </c>
       <c r="BO9" t="n">
-        <v>0.35608683236975</v>
+        <v>0.3668940743409324</v>
       </c>
       <c r="BP9" t="n">
-        <v>0.005068865814957325</v>
+        <v>0</v>
       </c>
       <c r="BQ9" t="n">
-        <v>0.1529829903340158</v>
+        <v>0.1675755632780588</v>
       </c>
       <c r="BR9" t="n">
-        <v>0.3487574031177041</v>
+        <v>0.3851287578467805</v>
       </c>
       <c r="BS9" t="n">
-        <v>0.000139366347672582</v>
+        <v>4.625346901017576e-05</v>
       </c>
       <c r="BT9" t="n">
-        <v>0.04840579710144927</v>
+        <v>0.05646631042973063</v>
       </c>
       <c r="BU9" t="n">
-        <v>0.4774866569626395</v>
+        <v>0.5655471289274107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>